<commit_message>
Clean up old test files and update test data
- Remove obsolete layout debug screenshots
- Remove old air_quality_stations.xlsx and test file
- Remove data.py helper script
- Update excel_container.xlsx with latest test data
- Update Claude Code settings

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/automation_script/excel_container.xlsx
+++ b/automation_script/excel_container.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AH12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1242,11 +1242,11 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Marquee Display</t>
+          <t>Vigilante AQS V2</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -1254,7 +1254,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>192.168.10.211</t>
+          <t>192.168.10.223</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -1263,7 +1263,7 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>00:01:C0:38:92:17</t>
+          <t>00:01:C0:38:91:B9</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1288,45 +1288,37 @@
       <c r="Q9" t="n">
         <v>0</v>
       </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>{'_id': '6786e056f5d136fafddd08a6', 'device_id': '6786e052f5d136fafddd08a0', 'network_type': 'DHCP', 'net_device_name': 'eth0', 'connection_name': 'Wired connection 1', 'forwarding': False, 'mac': '00:01:c0:38:92:17', 'address': '192.168.10.211', 'netmask': '255.255.255.0', 'gateway': '192.168.10.1', 'primary_dns': '192.168.10.5', 'secondary_dns': '192.168.10.6', 'tcpip': True, 'ethip': False, 'discovery': True, 'resetting': False, 'connected': True, 'created_date': '2025-01-14T22:08:18.990Z', 'modified_date': '2025-01-14T22:08:18.990Z', 'status': True, 'commTimeOut': '5000'}</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>{'lines': [{'_id': 1, 'line': 1, 'name': 'param1', 'unit': 'unit1', 'paramId': '-1', 'isUserText': False, 'userText': '', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': 'param1', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 2, 'line': 2, 'name': 'param2', 'unit': 'unit2', 'paramId': '-1', 'isUserText': False, 'userText': '', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': 'param2', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 3, 'line': 3, 'name': 'param3', 'unit': 'unit3', 'paramId': '-1', 'isUserText': False, 'userText': '', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': 'param3', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 4, 'line': 4, 'name': 'param4', 'unit': 'unit4', 'paramId': '-1', 'isUserText': False, 'userText': '', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': 'param4', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 5, 'line': 5, 'name': 'param5', 'unit': 'unit5', 'paramId': '-1', 'isUserText': False, 'userText': '', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': 'param5', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 6, 'line': 6, 'name': 'param6', 'unit': 'unit6', 'paramId': '-1', 'isUserText': False, 'userText': '', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': 'param6', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 7, 'line': 7, 'name': 'param7', 'unit': 'unit7', 'paramId': '-1', 'isUserText': False, 'userText': '', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': 'param7', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 8, 'line': 8, 'name': 'param8', 'unit': 'unit8', 'paramId': '-1', 'isUserText': False, 'userText': '', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': 'param8', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}], 'diagnostics_data': {'timeSinceLastPoll': '1124131.894', 'relayStatus': {'relay1': False, 'relay2': False, 'relay3': False}}, 'relay_config': [{'_id': 1, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}, {'_id': 2, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}, {'_id': 3, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}], '_id': '6786e052f5d136fafddd08a0', 'device_name': 'Marquee Display', 'location': '@Maestro', 'hardware_version': 1, 'software_version': 3.2, 'system_settings': {'timezone_offset': 5, 'history_length': 24, 'update_rate': 24, 'day_savings_offset': False, 'pause_rate': '03', 'keypad_dp': True, 'keypad_device_name': True, 'keypad_location': True, 'shift_length': 8, 'network_time': True, 'ntp_domain_name': '', 'custom_datetime': '2025-01-14T22:08:18.989Z', 'server_time': 24, 'ntp_server_address': 'time1.google.com'}, 'global_message_type': 'eip', 'global_message_web': {'_id': '6786e052f5d136fafddd08a1', 'text_line': '', 'colour': 'Amber', 'is_enabled': False, 'is_written': False, 'is_flashing': False}, 'global_message_eip': {'_id': '6786e052f5d136fafddd08a2', 'text_line': '', 'colour': 'Amber', 'is_enabled': False, 'is_written': False, 'is_flashing': False}, 'status': True}</t>
-        </is>
-      </c>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>MRQ05-Level 3000RAR-5435</t>
+          <t>AQI05-Level 3000RAR-SDFSF</t>
         </is>
       </c>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>5435</t>
+          <t>SDFSF</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr"/>
       <c r="AD9" t="inlineStr"/>
       <c r="AE9" s="2" t="n">
-        <v>45937.87853179398</v>
+        <v>45923.59818387732</v>
       </c>
       <c r="AF9" s="2" t="n">
-        <v>45938.77170657407</v>
+        <v>45937.63641530093</v>
       </c>
       <c r="AG9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH9" t="n">
         <v>1</v>
@@ -1334,11 +1326,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Vigilante AQS V2</t>
+          <t>Marquee Display</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -1346,7 +1338,7 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>192.168.10.223</t>
+          <t>192.168.10.211</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -1355,7 +1347,7 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>00:01:C0:38:91:B9</t>
+          <t>00:01:C0:38:92:17</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1380,37 +1372,43 @@
       <c r="Q10" t="n">
         <v>0</v>
       </c>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>{'_id': '6786e056f5d136fafddd08a6', 'device_id': '6786e052f5d136fafddd08a0', 'network_type': 'DHCP', 'net_device_name': 'eth0', 'connection_name': 'Wired connection 1', 'forwarding': False, 'mac': '00:01:c0:38:92:17', 'address': '192.168.10.211', 'netmask': '255.255.255.0', 'gateway': '192.168.10.1', 'primary_dns': '192.168.10.5', 'secondary_dns': '192.168.10.6', 'tcpip': True, 'ethip': False, 'discovery': True, 'resetting': False, 'connected': True, 'created_date': '2025-01-14T22:08:18.990Z', 'modified_date': '2025-01-14T22:08:18.990Z', 'status': True, 'commTimeOut': '5000'}</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>{'lines': [{'_id': 1, 'line': 1, 'name': 'param1', 'unit': 'unit1', 'paramId': '-1', 'isUserText': True, 'userText': 'HHHHHHHHHHH', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'userText', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 2, 'line': 2, 'name': 'param2', 'unit': 'unit2', 'paramId': '-1', 'isUserText': False, 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 3, 'line': 3, 'name': 'param3', 'unit': 'unit3', 'paramId': '-1', 'isUserText': False, 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 4, 'line': 4, 'name': 'param4', 'unit': 'unit4', 'paramId': '-1', 'isUserText': True, 'userText': 'HHHHHHHHHHH', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'userText', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 5, 'line': 5, 'name': 'param5', 'unit': 'unit5', 'paramId': '-1', 'isUserText': True, 'userText': 'HHHHHHHHHHH', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'userText', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 6, 'line': 6, 'name': 'param6', 'unit': 'unit6', 'paramId': '-1', 'isUserText': False, 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 7, 'line': 7, 'name': 'param7', 'unit': 'unit7', 'paramId': '-1', 'isUserText': False, 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}, {'_id': 8, 'line': 8, 'name': 'param8', 'unit': 'unit8', 'paramId': '-1', 'isUserText': True, 'userText': 'HHHHHHHHHHH', 'value': '0.0', 'color': 'Amber', 'isFlashing': False, 'format': '5.1', 'type': 'userText', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O2', 'flash': '^H0'}], 'diagnostics_data': {'timeSinceLastPoll': '1130889.568', 'relayStatus': {'relay1': False, 'relay2': False, 'relay3': False}}, 'relay_config': [{'_id': 1, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}, {'_id': 2, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}, {'_id': 3, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}], '_id': '6786e052f5d136fafddd08a0', 'device_name': 'Marquee Display', 'location': '@Maestro', 'hardware_version': 1, 'software_version': 3.2, 'system_settings': {'timezone_offset': 5, 'history_length': 24, 'update_rate': 24, 'day_savings_offset': False, 'pause_rate': '03', 'keypad_dp': True, 'keypad_device_name': True, 'keypad_location': True, 'shift_length': 8, 'network_time': True, 'ntp_domain_name': '', 'custom_datetime': '2025-01-14T22:08:18.989Z', 'server_time': 24, 'ntp_server_address': 'time1.google.com'}, 'global_message_type': 'eip', 'global_message_web': {'_id': '6786e052f5d136fafddd08a1', 'text_line': '', 'colour': 'Amber', 'is_enabled': False, 'is_written': False, 'is_flashing': False}, 'global_message_eip': {'_id': '6786e052f5d136fafddd08a2', 'text_line': '', 'colour': 'Amber', 'is_enabled': False, 'is_written': False, 'is_flashing': False}, 'status': True}</t>
+        </is>
+      </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
-      <c r="X10" t="n">
-        <v>3</v>
-      </c>
+      <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>AQI05-Level 3000RAR-SDFSF</t>
+          <t>MRQ05-Level 3000RAR-5435</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>SDFSF</t>
+          <t>5435</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr"/>
       <c r="AD10" t="inlineStr"/>
       <c r="AE10" s="2" t="n">
-        <v>45923.59818387732</v>
+        <v>45937.87853179398</v>
       </c>
       <c r="AF10" s="2" t="n">
-        <v>45937.63641530093</v>
+        <v>45938.84991699074</v>
       </c>
       <c r="AG10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH10" t="n">
         <v>1</v>
@@ -1418,11 +1416,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Vigilante AQS V2</t>
+          <t>Marquee Display</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -1430,7 +1428,7 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>192.168.10.222</t>
+          <t>192.168.10.61</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -1439,7 +1437,7 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>00:01:C0:38:92:0D</t>
+          <t>00:01:C0:2F:FB:08</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1464,37 +1462,45 @@
       <c r="Q11" t="n">
         <v>0</v>
       </c>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>{'_id': '67856a5c5846d03581a5fef6', 'device_id': '67856a585846d03581a5fef0', 'network_type': 'Static', 'net_device_name': 'eth0', 'connection_name': 'Wired connection 1', 'forwarding': False, 'mac': '00:01:C0:2F:FB:08', 'address': '192.168.10.61', 'netmask': '255.255.255.0', 'gateway': '192.168.10.1', 'primary_dns': '192.168.10.5', 'secondary_dns': '192.168.10.6', 'tcpip': True, 'ethip': False, 'discovery': True, 'resetting': False, 'connected': True, 'created_date': '2025-01-13T19:32:40.817Z', 'modified_date': '2025-01-13T19:32:40.817Z', 'status': True, 'commTimeOut': '5000'}</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>{'lines': [{'_id': 1, 'line': 1, 'name': 'A1-Vel', 'unit': 'ftmin', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '62.9', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': False, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 2, 'line': 2, 'name': 'A1-Vol', 'unit': 'kcfm', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '0.6', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': False, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 3, 'line': 3, 'name': 'CO', 'unit': 'ppm', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '0.0', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 4, 'line': 4, 'name': 'CO2', 'unit': '%', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '0.1', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 5, 'line': 5, 'name': 'A1-Mass', 'unit': 'lb/m', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '49.5', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 6, 'line': 6, 'name': 'Temp', 'unit': 'C', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '23.2', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 7, 'line': 7, 'name': 'Humidity', 'unit': '%', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '40.1', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 8, 'line': 8, 'name': 'BP', 'unit': 'kPa', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '99.6', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}], 'diagnostics_data': {'timeSinceLastPoll': '0.746', 'relayStatus': {'relay1': False, 'relay2': False, 'relay3': False}}, 'relay_config': [{'_id': 1, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}, {'_id': 2, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}, {'_id': 3, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}], '_id': '67856a585846d03581a5fef0', 'device_name': 'Marquee Display', 'location': '@Maestro', 'hardware_version': 1, 'software_version': 3.2, 'system_settings': {'timezone_offset': 5, 'history_length': 24, 'update_rate': 24, 'day_savings_offset': False, 'pause_rate': '03', 'keypad_dp': True, 'keypad_device_name': True, 'keypad_location': True, 'shift_length': 8, 'network_time': True, 'ntp_domain_name': '', 'custom_datetime': '2025-01-13T19:32:40.816Z', 'server_time': 24, 'ntp_server_address': 'time1.google.com'}, 'global_message_type': 'eip', 'global_message_web': {'_id': '67856a585846d03581a5fef1', 'text_line': '', 'colour': 'Amber', 'is_enabled': False, 'is_written': False, 'is_flashing': False}, 'global_message_eip': {'_id': '67856a585846d03581a5fef2', 'text_line': '', 'colour': 'Amber', 'is_enabled': False, 'is_written': False, 'is_flashing': False}, 'status': True}</t>
+        </is>
+      </c>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>AQI05-Level 3000RAR-ASSDF</t>
+          <t>MRQ05-Level 3000RAR-DSDS</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>ASSDF</t>
+          <t>DSDS</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr"/>
       <c r="AD11" t="inlineStr"/>
       <c r="AE11" s="2" t="n">
-        <v>45923.59826290509</v>
+        <v>45923.59722034722</v>
       </c>
       <c r="AF11" s="2" t="n">
-        <v>45937.6364153125</v>
+        <v>45938.84991804398</v>
       </c>
       <c r="AG11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH11" t="n">
         <v>1</v>
@@ -1502,11 +1508,11 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Marquee Display</t>
+          <t>ENG-VAQS1-33</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -1514,7 +1520,7 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>192.168.10.61</t>
+          <t>192.168.10.194</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -1523,7 +1529,7 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
-          <t>00:01:C0:2F:FB:08</t>
+          <t>00:1E:F8:00:10:3B</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1542,7 +1548,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Og==</t>
+          <t>YWRtaW46YWRtaW4=</t>
         </is>
       </c>
       <c r="Q12" t="n">
@@ -1550,149 +1556,57 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>{'_id': '67856a5c5846d03581a5fef6', 'device_id': '67856a585846d03581a5fef0', 'network_type': 'Static', 'net_device_name': 'eth0', 'connection_name': 'Wired connection 1', 'forwarding': False, 'mac': '00:01:C0:2F:FB:08', 'address': '192.168.10.61', 'netmask': '255.255.255.0', 'gateway': '192.168.10.1', 'primary_dns': '192.168.10.5', 'secondary_dns': '192.168.10.6', 'tcpip': True, 'ethip': False, 'discovery': True, 'resetting': False, 'connected': True, 'created_date': '2025-01-13T19:32:40.817Z', 'modified_date': '2025-01-13T19:32:40.817Z', 'status': True, 'commTimeOut': '5000'}</t>
+          <t>{}</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>{'lines': [{'_id': 1, 'line': 1, 'name': 'A1-Vel', 'unit': 'ftmin', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '49.2', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': False, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 2, 'line': 2, 'name': 'A1-Vol', 'unit': 'kcfm', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '0.5', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': False, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 3, 'line': 3, 'name': 'CO', 'unit': 'ppm', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '0.0', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 4, 'line': 4, 'name': 'CO2', 'unit': '%', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '0.1', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 5, 'line': 5, 'name': 'A1-Mass', 'unit': 'lb/m', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '38.6', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 6, 'line': 6, 'name': 'Temp', 'unit': 'C', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '23.2', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 7, 'line': 7, 'name': 'Humidity', 'unit': '%', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '39.2', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}, {'_id': 8, 'line': 8, 'name': 'BP', 'unit': 'kPa', 'paramId': '-1', 'isUserText': False, 'userText': 'HHHHHHHHHHHHHHHHHHHH', 'value': '99.6', 'color': 'Green', 'isFlashing': False, 'format': '5.1', 'type': 'parameter', 'deviceName': 'Marquee Display', 'dynamicText': '', 'isEnable': True, 'isTimeoutEnabled': True, 'lineColorFlashSource': 'modbus', 'lineErrorText': '***', 'isFailColorSourceWeb': True, 'lineColor': '^O1', 'flash': '^H0'}], 'diagnostics_data': {'timeSinceLastPoll': '0.424', 'relayStatus': {'relay1': False, 'relay2': False, 'relay3': False}}, 'relay_config': [{'_id': 1, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}, {'_id': 2, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}, {'_id': 3, 'isPulse': False, 'time': '5000', 'failureMode': 'failOpen', 'value': False, 'valuem': False}], '_id': '67856a585846d03581a5fef0', 'device_name': 'Marquee Display', 'location': '@Maestro', 'hardware_version': 1, 'software_version': 3.2, 'system_settings': {'timezone_offset': 5, 'history_length': 24, 'update_rate': 24, 'day_savings_offset': False, 'pause_rate': '03', 'keypad_dp': True, 'keypad_device_name': True, 'keypad_location': True, 'shift_length': 8, 'network_time': True, 'ntp_domain_name': '', 'custom_datetime': '2025-01-13T19:32:40.816Z', 'server_time': 24, 'ntp_server_address': 'time1.google.com'}, 'global_message_type': 'eip', 'global_message_web': {'_id': '67856a585846d03581a5fef1', 'text_line': '', 'colour': 'Amber', 'is_enabled': False, 'is_written': False, 'is_flashing': False}, 'global_message_eip': {'_id': '67856a585846d03581a5fef2', 'text_line': '', 'colour': 'Amber', 'is_enabled': False, 'is_written': False, 'is_flashing': False}, 'status': True}</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr"/>
+          <t>{'network': {}, 'ports': {'configured_ports': {}}, 'protocol': {}, 'marquee': {}, 'time': {'formatted_date': None}, 'board': {}, 'gas_sensor_1': {}, 'gas_sensor_2': {}, 'diagnostic': {'Device': {'buildDate': 'Apr 14 2022 13:38:59', 'version': 'v4.21', 'macAddress': '00:1E:F8:00:10:3B', 'iPAddress': '192.168.10.194', 'deviceName': 'ENG-VAQS1-33', '': ''}, 'Status': {'lastReset': '01/02/00  20:00:00', 'boardTemp': '35.5  C', 'pollTimer': '1967', 'errorCode': '30', '': ''}}, 'airconf_1': {}, 'airconf_2': {}, 'analog_out': {}, 'analog_out_test': {}, 'analog_out_relays': {}, 'climate_ptx': {}, 'ad4_1': {}, 'ad4_2': {}, 'device_version': {'hardware_version': '3', 'software_version': 'v4.21'}}</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>{'sensor_diagnostics': {'airflow': [{'name': 'af1', 'status': {'message': 'Not Installed', 'state': 'Not Installed'}, 'com_status1': 'Error', 'com_status2': 'Error', 'pulse_quality1': ' 0 %', 'pulse_quality2': ' 0 %', 'transit_time1': '6042 uS', 'transit_time2': '6042 uS', 'receive_count1': ' 0', 'receive_count2': ' 0', 'receive_miss1': ' 0', 'receive_miss2': ' 0', 'voltage1': 0, 'voltage2': 0, 'temperature1': 0, 'temperature2': 0}, {'name': 'af2', 'status': {'message': 'Not Installed', 'state': 'Not Installed'}, 'com_status1': 'Error', 'com_status2': 'Error', 'pulse_quality1': ' 0 %', 'pulse_quality2': ' 0 %', 'transit_time1': '6042 uS', 'transit_time2': '6042 uS', 'receive_count1': ' 0', 'receive_count2': ' 0', 'receive_miss1': ' 0', 'receive_miss2': ' 0', 'voltage1': 0, 'voltage2': 0, 'temperature1': 0, 'temperature2': 0}, {'name': 'af3', 'status': {'message': 'Not Installed', 'state': 'Not Installed'}, 'com_status1': 'Error', 'com_status2': 'Error', 'pulse_quality1': ' 0 %', 'pulse_quality2': ' 0 %', 'transit_time1': '6042 uS', 'transit_time2': '6042 uS', 'receive_count1': ' 0', 'receive_count2': ' 0', 'receive_miss1': ' 0', 'receive_miss2': ' 0', 'voltage1': 0, 'voltage2': 0, 'temperature1': 0, 'temperature2': 0}, {'name': 'af4', 'status': {'message': 'Not Installed', 'state': 'Not Installed'}, 'com_status1': 'Error', 'com_status2': 'Error', 'pulse_quality1': ' 0 %', 'pulse_quality2': ' 0 %', 'transit_time1': '6042 uS', 'transit_time2': '6042 uS', 'receive_count1': ' 0', 'receive_count2': ' 0', 'receive_miss1': ' 0', 'receive_miss2': ' 0', 'voltage1': 0, 'voltage2': 0, 'temperature1': 0, 'temperature2': 0}], 'gas': [{'name': 'gas1', 'message': 'Span Cal Fault', 'status_msg': '0x0003', 'value': '1.00', 'stel': '33.80', 'twa': '33.80', 'caldate': '22/02/2023', 'factdate': '00/00/2000', 'status_hex': '0x0003', 'span_gas': '1 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '7934', 'temperature': '33.80', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '22/02/2023'}, {'name': 'gas2', 'message': 'Sensor Missing', 'status_msg': '0x8000', 'value': '0.00', 'stel': '0.00', 'twa': '0.00', 'caldate': '...', 'factdate': '...', 'status_hex': '0x8000', 'span_gas': '0 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '0', 'temperature': '0.00', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '...'}, {'name': 'gas3', 'message': 'Not Configured', 'status_msg': '0x0000', 'value': '0.00', 'stel': '0.00', 'twa': '0.00', 'caldate': '...', 'factdate': '...', 'status_hex': '0x0000', 'span_gas': '0 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '0', 'temperature': '0.00', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '...'}, {'name': 'gas4', 'message': 'Not Configured', 'status_msg': '0x0000', 'value': '0.00', 'stel': '0.00', 'twa': '0.00', 'caldate': '...', 'factdate': '...', 'status_hex': '0x0000', 'span_gas': '0 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '0', 'temperature': '0.00', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '...'}, {'name': 'gas5', 'message': 'Not Configured', 'status_msg': '0x0000', 'value': '0.00', 'stel': '0.00', 'twa': '0.00', 'caldate': '...', 'factdate': '...', 'status_hex': '0x0000', 'span_gas': '0 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '0', 'temperature': '0.00', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '...'}, {'name': 'gas6', 'message': 'Not Configured', 'status_msg': '0x0000', 'value': '0.00', 'stel': '0.00', 'twa': '0.00', 'caldate': '...', 'factdate': '...', 'status_hex': '0x0000', 'span_gas': '0 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '0', 'temperature': '0.00', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '...'}], 'board': [{'temp': '35.7 °C', 'poll_time': ' 2253 seconds'}]}}</t>
+        </is>
+      </c>
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>MRQ05-Level 3000RAR-DSDS</t>
-        </is>
-      </c>
-      <c r="Z12" t="inlineStr"/>
+          <t>AQI02-Level 3000RAR-34</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>DSDS</t>
+          <t>34</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr"/>
-      <c r="AD12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
       <c r="AE12" s="2" t="n">
-        <v>45923.59722034722</v>
+        <v>45937.63640270833</v>
       </c>
       <c r="AF12" s="2" t="n">
-        <v>45938.77171016204</v>
+        <v>45938.8498596412</v>
       </c>
       <c r="AG12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AH12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>10</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>ENG-VAQS1-33</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>192.168.10.194</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>00:1E:F8:00:10:3B</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>edfdc8a8-d692-4bd4-8050-641b0c25518e</t>
-        </is>
-      </c>
-      <c r="M13" t="b">
-        <v>0</v>
-      </c>
-      <c r="N13" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13" t="b">
-        <v>0</v>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>YWRtaW46YWRtaW4=</t>
-        </is>
-      </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>{}</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>{'network': {}, 'ports': {'configured_ports': {}}, 'protocol': {}, 'marquee': {}, 'time': {'formatted_date': None}, 'board': {}, 'gas_sensor_1': {}, 'gas_sensor_2': {}, 'diagnostic': {'Device': {'buildDate': 'Apr 14 2022 13:38:59', 'version': 'v4.21', 'macAddress': '00:1E:F8:00:10:3B', 'iPAddress': '192.168.10.194', 'deviceName': 'ENG-VAQS1-33', '': ''}, 'Status': {'lastReset': '01/02/00  20:00:00', 'boardTemp': '33.5  C', 'pollTimer': '3750', 'errorCode': '30', '': ''}}, 'airconf_1': {}, 'airconf_2': {}, 'analog_out': {}, 'analog_out_test': {}, 'analog_out_relays': {}, 'climate_ptx': {}, 'ad4_1': {}, 'ad4_2': {}, 'device_version': {'hardware_version': '3', 'software_version': 'v4.21'}}</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>{'sensor_diagnostics': {'airflow': [{'name': 'af1', 'status': {'message': 'Not Installed', 'state': 'Not Installed'}, 'com_status1': 'Error', 'com_status2': 'Error', 'pulse_quality1': ' 0 %', 'pulse_quality2': ' 0 %', 'transit_time1': '6042 uS', 'transit_time2': '6042 uS', 'receive_count1': ' 0', 'receive_count2': ' 0', 'receive_miss1': ' 0', 'receive_miss2': ' 0', 'voltage1': 0, 'voltage2': 0, 'temperature1': 0, 'temperature2': 0}, {'name': 'af2', 'status': {'message': 'Not Installed', 'state': 'Not Installed'}, 'com_status1': 'Error', 'com_status2': 'Error', 'pulse_quality1': ' 0 %', 'pulse_quality2': ' 0 %', 'transit_time1': '6042 uS', 'transit_time2': '6042 uS', 'receive_count1': ' 0', 'receive_count2': ' 0', 'receive_miss1': ' 0', 'receive_miss2': ' 0', 'voltage1': 0, 'voltage2': 0, 'temperature1': 0, 'temperature2': 0}, {'name': 'af3', 'status': {'message': 'Not Installed', 'state': 'Not Installed'}, 'com_status1': 'Error', 'com_status2': 'Error', 'pulse_quality1': ' 0 %', 'pulse_quality2': ' 0 %', 'transit_time1': '6042 uS', 'transit_time2': '6042 uS', 'receive_count1': ' 0', 'receive_count2': ' 0', 'receive_miss1': ' 0', 'receive_miss2': ' 0', 'voltage1': 0, 'voltage2': 0, 'temperature1': 0, 'temperature2': 0}, {'name': 'af4', 'status': {'message': 'Not Installed', 'state': 'Not Installed'}, 'com_status1': 'Error', 'com_status2': 'Error', 'pulse_quality1': ' 0 %', 'pulse_quality2': ' 0 %', 'transit_time1': '6042 uS', 'transit_time2': '6042 uS', 'receive_count1': ' 0', 'receive_count2': ' 0', 'receive_miss1': ' 0', 'receive_miss2': ' 0', 'voltage1': 0, 'voltage2': 0, 'temperature1': 0, 'temperature2': 0}], 'gas': [{'name': 'gas1', 'message': 'Span Cal Fault', 'status_msg': '0x0003', 'value': '1.00', 'stel': '33.20', 'twa': '33.20', 'caldate': '22/02/2023', 'factdate': '00/00/2000', 'status_hex': '0x0003', 'span_gas': '1 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '7934', 'temperature': '33.20', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '22/02/2023'}, {'name': 'gas2', 'message': 'Sensor Missing', 'status_msg': '0x8000', 'value': '0.00', 'stel': '0.00', 'twa': '0.00', 'caldate': '...', 'factdate': '...', 'status_hex': '0x8000', 'span_gas': '0 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '0', 'temperature': '0.00', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '...'}, {'name': 'gas3', 'message': 'Not Configured', 'status_msg': '0x0000', 'value': '0.00', 'stel': '0.00', 'twa': '0.00', 'caldate': '...', 'factdate': '...', 'status_hex': '0x0000', 'span_gas': '0 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '0', 'temperature': '0.00', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '...'}, {'name': 'gas4', 'message': 'Not Configured', 'status_msg': '0x0000', 'value': '0.00', 'stel': '0.00', 'twa': '0.00', 'caldate': '...', 'factdate': '...', 'status_hex': '0x0000', 'span_gas': '0 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '0', 'temperature': '0.00', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '...'}, {'name': 'gas5', 'message': 'Not Configured', 'status_msg': '0x0000', 'value': '0.00', 'stel': '0.00', 'twa': '0.00', 'caldate': '...', 'factdate': '...', 'status_hex': '0x0000', 'span_gas': '0 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '0', 'temperature': '0.00', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '...'}, {'name': 'gas6', 'message': 'Not Configured', 'status_msg': '0x0000', 'value': '0.00', 'stel': '0.00', 'twa': '0.00', 'caldate': '...', 'factdate': '...', 'status_hex': '0x0000', 'span_gas': '0 ppm', 'hw_version': '', 'sw_version': '', 'remote_board_sw_version': '', 'serial_number': '0', 'temperature': '0.00', 'temperature_unit': 'C', 'cal_timer': '0', 'last_cal_date': '...'}], 'board': [{'temp': '34.3 °C', 'poll_time': ' 4323 seconds'}]}}</t>
-        </is>
-      </c>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>AQI02-Level 3000RAR-34</t>
-        </is>
-      </c>
-      <c r="Z13" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="AE13" s="2" t="n">
-        <v>45937.63640270833</v>
-      </c>
-      <c r="AF13" s="2" t="n">
-        <v>45938.77170653935</v>
-      </c>
-      <c r="AG13" t="n">
-        <v>5</v>
-      </c>
-      <c r="AH13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1915,7 +1829,7 @@
         <v>45931.76653497685</v>
       </c>
       <c r="Q3" s="2" t="n">
-        <v>45938.77169328704</v>
+        <v>45938.84990244213</v>
       </c>
       <c r="R3" t="n">
         <v>8</v>
@@ -1983,7 +1897,7 @@
         <v>45937.63648284722</v>
       </c>
       <c r="Q4" s="2" t="n">
-        <v>45938.77170584491</v>
+        <v>45938.84985421296</v>
       </c>
       <c r="R4" t="n">
         <v>10</v>
@@ -1991,34 +1905,34 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fd5adb3c-a592-417c-90bb-4fcc93e99496</t>
+          <t>vaqs1-integral_climate-10-1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>{'id': 'fd5adb3c-a592-417c-90bb-4fcc93e99496', 'board': 0, 'subport': 0, 'local_board': '', 'remote': False, 'name': 'Climate Sensor', 'location': 'Integral', 'temperature_unit': '', 'humidity_unit': '', 'pressure_unit': '', 'wbgt_calculation': 'US', 'temperature_offset': 0, 'humidity_offset': 0, 'pressure_offset': 0, 'error_timeout': 60}</t>
+          <t>{}</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -2028,118 +1942,116 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
         <v>3</v>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
-        <v>333333</v>
+        <v>3333</v>
       </c>
       <c r="N5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>['Temp', 'Humidity', 'Wet Bulb']</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O5" t="inlineStr"/>
       <c r="P5" s="2" t="n">
-        <v>45923.59826671296</v>
+        <v>45937.63648418982</v>
       </c>
       <c r="Q5" s="2" t="n">
-        <v>45925.57786405092</v>
+        <v>45938.84985542824</v>
       </c>
       <c r="R5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>vaqs1-integral_climate-10-1</t>
+          <t>7b4eeeec-e8da-422c-8e45-19ea1e38c737</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>ttymxc5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>{'id': '7b4eeeec-e8da-422c-8e45-19ea1e38c737', 'local_board': 'ttymxc5', 'board': 0, 'subport': 1, 'remote': False, 'name': 'Gas', 'location': '1800L_RAR', 'gas_sensor_type': 17, 'error_timeout': 5, 'alarms': 'High', 'inst_warning': 5, 'stel_warning': 0, 'twa_warning': 0, 'inst_alarm': 7, 'stel_alarm': 0, 'twa_alarm': 0, 'inst_enable': True, 'stel_enable': False, 'twa_enable': False, 'configured': False}</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Integral</t>
+          <t>1800L_RAR</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
-      </c>
-      <c r="L6" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="L6" t="n">
+        <v>17</v>
+      </c>
       <c r="M6" t="n">
-        <v>3333</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" s="2" t="n">
-        <v>45937.63648418982</v>
+        <v>45923.59716788195</v>
       </c>
       <c r="Q6" s="2" t="n">
-        <v>45938.77170708333</v>
+        <v>45938.84991282407</v>
       </c>
       <c r="R6" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>15</v>
+      </c>
+      <c r="B7" t="n">
         <v>9</v>
       </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7b4eeeec-e8da-422c-8e45-19ea1e38c737</t>
+          <t>fd5adb3c-a592-417c-90bb-4fcc93e99496</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ttymxc5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -2149,17 +2061,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>{'id': '7b4eeeec-e8da-422c-8e45-19ea1e38c737', 'local_board': 'ttymxc5', 'board': 0, 'subport': 1, 'remote': False, 'name': 'Gas', 'location': '1800L_RAR', 'gas_sensor_type': 17, 'error_timeout': 5, 'alarms': 'High', 'inst_warning': 5, 'stel_warning': 0, 'twa_warning': 0, 'inst_alarm': 7, 'stel_alarm': 0, 'twa_alarm': 0, 'inst_enable': True, 'stel_enable': False, 'twa_enable': False, 'configured': False}</t>
+          <t>{'id': 'fd5adb3c-a592-417c-90bb-4fcc93e99496', 'board': 0, 'subport': 0, 'local_board': '', 'remote': False, 'name': 'Climate Sensor', 'location': 'Integral', 'temperature_unit': '', 'humidity_unit': '', 'pressure_unit': '', 'wbgt_calculation': 'US', 'temperature_offset': 0, 'humidity_offset': 0, 'pressure_offset': 0, 'error_timeout': 60}</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1800L_RAR</t>
+          <t>Integral</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -2171,27 +2083,27 @@
         <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>2</v>
-      </c>
-      <c r="L7" t="n">
-        <v>17</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>333333</v>
       </c>
       <c r="N7" t="n">
         <v>1</v>
       </c>
-      <c r="O7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>['Temp', 'Humidity', 'Wet Bulb']</t>
+        </is>
+      </c>
       <c r="P7" s="2" t="n">
-        <v>45923.59716788195</v>
+        <v>45923.59826671296</v>
       </c>
       <c r="Q7" s="2" t="n">
-        <v>45938.7717087963</v>
-      </c>
-      <c r="R7" t="n">
-        <v>5</v>
-      </c>
+        <v>45925.57786405092</v>
+      </c>
+      <c r="R7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -2257,7 +2169,7 @@
         <v>45923.5971237037</v>
       </c>
       <c r="Q8" s="2" t="n">
-        <v>45938.77169027778</v>
+        <v>45938.84990292824</v>
       </c>
       <c r="R8" t="n">
         <v>4</v>
@@ -2325,7 +2237,7 @@
         <v>45923.59712486111</v>
       </c>
       <c r="Q9" s="2" t="n">
-        <v>45938.77169141204</v>
+        <v>45938.84990407407</v>
       </c>
       <c r="R9" t="n">
         <v>4</v>
@@ -2391,7 +2303,7 @@
         <v>45933.63285299768</v>
       </c>
       <c r="Q10" s="2" t="n">
-        <v>45938.77170876157</v>
+        <v>45938.84991278935</v>
       </c>
       <c r="R10" t="n">
         <v>5</v>
@@ -2459,9 +2371,7 @@
       <c r="Q11" s="2" t="n">
         <v>45925.57786505787</v>
       </c>
-      <c r="R11" t="n">
-        <v>9</v>
-      </c>
+      <c r="R11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -2525,7 +2435,7 @@
         <v>45924.61827726852</v>
       </c>
       <c r="Q12" s="2" t="n">
-        <v>45938.77170878472</v>
+        <v>45938.84991280093</v>
       </c>
       <c r="R12" t="n">
         <v>5</v>
@@ -2593,7 +2503,7 @@
         <v>45923.59712491898</v>
       </c>
       <c r="Q13" s="2" t="n">
-        <v>45938.77169145834</v>
+        <v>45938.84990412037</v>
       </c>
       <c r="R13" t="n">
         <v>4</v>
@@ -2661,7 +2571,7 @@
         <v>45923.59712489583</v>
       </c>
       <c r="Q14" s="2" t="n">
-        <v>45938.77169144676</v>
+        <v>45938.84990409722</v>
       </c>
       <c r="R14" t="n">
         <v>4</v>
@@ -2729,7 +2639,7 @@
         <v>45923.59712488426</v>
       </c>
       <c r="Q15" s="2" t="n">
-        <v>45938.77169142361</v>
+        <v>45938.84990408565</v>
       </c>
       <c r="R15" t="n">
         <v>4</v>
@@ -2799,7 +2709,7 @@
         <v>45923.59716686342</v>
       </c>
       <c r="Q16" s="2" t="n">
-        <v>45938.77170810185</v>
+        <v>45938.84991185185</v>
       </c>
       <c r="R16" t="n">
         <v>5</v>

</xml_diff>